<commit_message>
industrial elec demand reduced
</commit_message>
<xml_diff>
--- a/data/haag/data.xlsx
+++ b/data/haag/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -1240,7 +1240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2236,11 +2236,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2324,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="27">
-        <v>0.95</v>
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
made timestep 'scale' commodity-dependent
</commit_message>
<xml_diff>
--- a/data/haag/data.xlsx
+++ b/data/haag/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
   <si>
     <t>Commodity</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>weight</t>
-  </si>
-  <si>
-    <t>scale</t>
   </si>
   <si>
     <t>peak</t>
@@ -312,9 +309,6 @@
   </si>
   <si>
     <t>t high</t>
-  </si>
-  <si>
-    <t>hours</t>
   </si>
 </sst>
 </file>
@@ -907,7 +901,7 @@
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
       <c r="C3" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -920,7 +914,7 @@
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
       <c r="C4" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
@@ -955,7 +949,7 @@
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="21"/>
       <c r="C7" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -968,11 +962,11 @@
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="21"/>
       <c r="C8" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -983,11 +977,11 @@
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
       <c r="C9" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -998,11 +992,11 @@
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
       <c r="C10" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1013,11 +1007,11 @@
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -1028,11 +1022,11 @@
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="21"/>
       <c r="C12" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1054,7 +1048,7 @@
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="C14" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -1067,11 +1061,11 @@
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -1082,11 +1076,11 @@
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -1097,11 +1091,11 @@
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -1244,7 +1238,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,10 +1267,10 @@
         <v>9</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>18</v>
@@ -1342,16 +1336,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="3">
-        <v>1500</v>
+        <v>350</v>
       </c>
       <c r="D4" s="3">
-        <v>0.01</v>
+        <v>2E-3</v>
       </c>
       <c r="E4" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F4" s="10">
-        <v>1</v>
+        <v>1.5E-3</v>
       </c>
       <c r="G4" s="10">
         <v>2.0000000000000002E-5</v>
@@ -1377,7 +1371,7 @@
         <v>0.08</v>
       </c>
       <c r="F5" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="10">
         <v>1.6000000000000001E-4</v>
@@ -1420,7 +1414,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -1460,11 +1454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,64 +1490,64 @@
         <v>18</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="35">
-        <v>10000</v>
+        <v>800</v>
       </c>
       <c r="C2" s="3">
-        <v>0.2</v>
+        <v>1.5</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
       </c>
       <c r="E2" s="35">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="F2" s="35">
         <v>600000</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="35">
-        <v>15000</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="3">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
       </c>
       <c r="E3" s="35">
-        <v>100</v>
+        <v>5000</v>
       </c>
       <c r="F3" s="35">
         <v>600000</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="35">
         <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>0.2</v>
+        <v>3.5</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -1562,90 +1556,90 @@
         <v>0</v>
       </c>
       <c r="F4" s="35">
-        <v>1000</v>
+        <v>6000</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="35">
-        <v>5000</v>
+        <v>500</v>
       </c>
       <c r="C5" s="3">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="35">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F5" s="35">
         <v>150000</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="35">
-        <v>8000</v>
+        <v>800</v>
       </c>
       <c r="C6" s="3">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
       </c>
       <c r="E6" s="35">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="F6" s="35">
         <v>400000</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="35">
-        <v>5000</v>
+        <v>700</v>
       </c>
       <c r="C7" s="3">
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
       <c r="E7" s="35">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="F7" s="35">
-        <v>999990</v>
+        <v>150000</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="35">
         <v>0</v>
       </c>
       <c r="C8" s="3">
-        <v>0.3</v>
+        <v>3.5</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1654,21 +1648,21 @@
         <v>0</v>
       </c>
       <c r="F8" s="35">
-        <v>1000</v>
+        <v>6000</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="35">
-        <v>9000</v>
+        <v>900</v>
       </c>
       <c r="C9" s="3">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -1680,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1704,7 +1698,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3:D4"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,7 +1725,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1745,7 +1739,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1759,7 +1753,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1773,7 +1767,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -1787,7 +1781,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
@@ -1801,7 +1795,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -1815,7 +1809,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -1824,12 +1818,12 @@
         <v>13</v>
       </c>
       <c r="D8" s="8">
-        <v>0.7</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -1843,7 +1837,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
@@ -1857,7 +1851,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -1871,7 +1865,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
@@ -1885,7 +1879,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>4</v>
@@ -1899,7 +1893,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
@@ -1913,7 +1907,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>2</v>
@@ -1927,7 +1921,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
@@ -1941,7 +1935,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -1955,7 +1949,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -1969,7 +1963,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
@@ -1983,7 +1977,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>1</v>
@@ -1997,7 +1991,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -2011,7 +2005,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
@@ -2025,10 +2019,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -2039,7 +2033,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
@@ -2053,7 +2047,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>2</v>
@@ -2067,7 +2061,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
@@ -2131,13 +2125,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,7 +2142,7 @@
     <col min="4" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2156,77 +2150,82 @@
         <v>20</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" s="35">
-        <f>D2</f>
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
       </c>
-      <c r="D2" s="35">
-        <v>60</v>
-      </c>
-      <c r="G2" s="35"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="35"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="35">
-        <f>D3</f>
         <v>1000</v>
       </c>
       <c r="C3" s="8">
         <v>0.8</v>
       </c>
-      <c r="D3" s="35">
-        <v>1000</v>
-      </c>
-      <c r="G3" s="35"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D3" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="35">
+        <v>2700</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="35"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="35">
-        <f>D4</f>
-        <v>2700</v>
-      </c>
-      <c r="C4" s="8">
-        <v>0.65</v>
-      </c>
-      <c r="D4" s="35">
-        <v>2700</v>
-      </c>
-      <c r="G4" s="35"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="B5" s="35">
-        <f>D5</f>
-        <v>5000</v>
+        <v>5040</v>
       </c>
       <c r="C5" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="D5" s="35">
-        <v>5000</v>
-      </c>
-      <c r="G5" s="35"/>
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="F5" s="35"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="35"/>
+      <c r="D6" s="8"/>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Scaling factor Elec (1)" prompt="Relative scaling factor of demand 'Elec' per time step. Interpret like y-values of a normalised annual load duration curve." sqref="C1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Scaling factor Heat (1)" prompt="Relative scaling factor of demand 'Heat' per time step. Interpret like y-values of a normalised annual load duration curve." sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Timestep weight (hours)" prompt="Length of timestep in hours. Sum of all weights == 8760" sqref="B1"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2236,11 +2235,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,18 +2251,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -2274,7 +2273,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -2285,7 +2284,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -2296,18 +2295,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="27">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -2318,7 +2317,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -2329,18 +2328,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="27">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
district * plant fixed invest cost from 5000 to 15000; minor runhaag.py improvements
</commit_message>
<xml_diff>
--- a/data/haag/data.xlsx
+++ b/data/haag/data.xlsx
@@ -1458,7 +1458,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="35">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="F2" s="35">
         <v>600000</v>
@@ -1530,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="35">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="F3" s="35">
         <v>600000</v>

</xml_diff>

<commit_message>
completed column comments in data.xlsx
</commit_message>
<xml_diff>
--- a/data/haag/data.xlsx
+++ b/data/haag/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1238,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,6 +1445,14 @@
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€/m)" prompt="Capacity-independent investment costs for pipe/cable to transmit that commodity." sqref="C1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable invest costs (€/kW/m)" prompt="Capacity-dependent investment costs for transmission capacity of a commodity from one vertex to another." sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Purchase costs (€/kWh)" prompt="Cost for buying that commodity at source vertices, if any exist in the vertex_shapefile." sqref="E1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed loss fraction (kW/m)" prompt="Powerflow-independent loss of energy per meter of transmission length through the network. The fixed loss is calculated by (length * loss-fix)." sqref="F1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable power loss (1/kW/m)" prompt="Relative loss term, dependent on input power flow through a &quot;pipe&quot;:_x000a_Ingoing power flow per edge is multiplied by (1 - length * loss-var)" sqref="G1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Maximum possible transmission capacity per edge." sqref="H1"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1454,11 +1462,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,7 +1706,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,7 +2139,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2239,7 +2247,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2354,6 +2362,9 @@
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Building peak demand (kW/m²)" prompt="Peak demand of building type (must be present in building_shapefile) normalised to building area. Annual demand is encoded in timestep weights on sheet Time." sqref="C1"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added attribute allowed-max + constraint
</commit_message>
<xml_diff>
--- a/data/haag/data.xlsx
+++ b/data/haag/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="72">
   <si>
     <t>Commodity</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>t high</t>
+  </si>
+  <si>
+    <t>allowed-max</t>
+  </si>
+  <si>
+    <t>inf</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,12 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+    </dxf>
     <dxf>
       <border>
         <top style="thin">
@@ -877,7 +888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1232,13 +1243,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,10 +1258,12 @@
     <col min="2" max="4" width="11.42578125" style="3"/>
     <col min="5" max="5" width="11.42578125" style="6"/>
     <col min="6" max="7" width="11.42578125" style="10"/>
-    <col min="8" max="16384" width="11.42578125" style="3"/>
+    <col min="8" max="8" width="11.42578125" style="3"/>
+    <col min="9" max="9" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1275,8 +1288,11 @@
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1301,8 +1317,12 @@
       <c r="H2" s="3">
         <v>750000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="31" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1327,8 +1347,12 @@
       <c r="H3" s="3">
         <v>500000</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="31" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1353,8 +1377,12 @@
       <c r="H4" s="3">
         <v>160000</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="31" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1379,8 +1407,12 @@
       <c r="H5" s="3">
         <v>90000</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="31" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1411,8 +1443,11 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
@@ -1438,20 +1473,25 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="I7" s="31" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsErrors" dxfId="3" priority="1">
+    <cfRule type="containsErrors" dxfId="4" priority="1">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€/m)" prompt="Capacity-independent investment costs for pipe/cable to transmit that commodity." sqref="C1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable invest costs (€/kW/m)" prompt="Capacity-dependent investment costs for transmission capacity of a commodity from one vertex to another." sqref="D1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Purchase costs (€/kWh)" prompt="Cost for buying that commodity at source vertices, if any exist in the vertex_shapefile." sqref="E1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed loss fraction (kW/m)" prompt="Powerflow-independent loss of energy per meter of transmission length through the network. The fixed loss is calculated by (length * loss-fix)." sqref="F1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable power loss (1/kW/m)" prompt="Relative loss term, dependent on input power flow through a &quot;pipe&quot;:_x000a_Ingoing power flow per edge is multiplied by (1 - length * loss-var)" sqref="G1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Maximum possible transmission capacity per edge." sqref="H1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum allowed generation" prompt="Limits the net amount of generation of this commodity (e.g. CO2). Note that processes that consume a commodity (e.g. CCS) can reduce the net amount." sqref="I1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2097,10 +2137,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>EXACT("In", INDIRECT("Z"&amp;ROW()&amp;"S3",FALSE()))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2358,7 +2398,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add cost-fix to rivus.py and all sample inputs
</commit_message>
<xml_diff>
--- a/data/haag/data.xlsx
+++ b/data/haag/data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdorfner\Documents\Themen\Thesis\Modelle\rivus\data\haag\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -14,12 +19,12 @@
     <sheet name="Time" sheetId="5" r:id="rId5"/>
     <sheet name="Area-Demand" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
   <si>
     <t>Commodity</t>
   </si>
@@ -315,6 +320,9 @@
   </si>
   <si>
     <t>inf</t>
+  </si>
+  <si>
+    <t>cost-fix</t>
   </si>
 </sst>
 </file>
@@ -554,12 +562,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color theme="5" tint="0.59996337778862885"/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <border>
         <top style="thin">
@@ -595,14 +598,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -640,9 +646,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -677,7 +683,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -712,7 +718,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1243,27 +1249,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="4" width="11.42578125" style="3"/>
-    <col min="5" max="5" width="11.42578125" style="6"/>
-    <col min="6" max="7" width="11.42578125" style="10"/>
-    <col min="8" max="8" width="11.42578125" style="3"/>
-    <col min="9" max="9" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="3"/>
+    <col min="2" max="5" width="11.42578125" style="3"/>
+    <col min="6" max="6" width="11.42578125" style="6"/>
+    <col min="7" max="8" width="11.42578125" style="10"/>
+    <col min="9" max="9" width="11.42578125" style="3"/>
+    <col min="10" max="10" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1276,23 +1282,26 @@
       <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1305,24 +1314,27 @@
       <c r="D2" s="3">
         <v>1E-3</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
         <v>0.3</v>
       </c>
-      <c r="F2" s="10">
+      <c r="G2" s="10">
         <v>1E-3</v>
       </c>
-      <c r="G2" s="10">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
         <v>750000</v>
       </c>
-      <c r="I2" s="31" t="e">
+      <c r="J2" s="31" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1335,24 +1347,27 @@
       <c r="D3" s="3">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
         <v>0.35</v>
       </c>
-      <c r="F3" s="10">
+      <c r="G3" s="10">
         <v>1E-4</v>
       </c>
-      <c r="G3" s="10">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
         <v>500000</v>
       </c>
-      <c r="I3" s="31" t="e">
+      <c r="J3" s="31" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1365,24 +1380,27 @@
       <c r="D4" s="3">
         <v>2E-3</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F4" s="10">
+      <c r="G4" s="10">
         <v>1.5E-3</v>
       </c>
-      <c r="G4" s="10">
+      <c r="H4" s="10">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>160000</v>
       </c>
-      <c r="I4" s="31" t="e">
+      <c r="J4" s="31" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1395,24 +1413,27 @@
       <c r="D5" s="3">
         <v>0.01</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
         <v>0.08</v>
       </c>
-      <c r="F5" s="10">
+      <c r="G5" s="10">
         <v>1</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="10">
         <v>1.6000000000000001E-4</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>90000</v>
       </c>
-      <c r="I5" s="31" t="e">
+      <c r="J5" s="31" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1427,11 +1448,11 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="E6" s="32" t="e">
+      <c r="E6" s="31" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="F6" s="33" t="e">
+      <c r="F6" s="32" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
@@ -1439,15 +1460,19 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="H6" s="31" t="e">
+      <c r="H6" s="33" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="31" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
@@ -1460,38 +1485,41 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
         <v>0.01</v>
       </c>
-      <c r="F7" s="10">
-        <v>0</v>
-      </c>
       <c r="G7" s="10">
         <v>0</v>
       </c>
-      <c r="H7" s="31" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="H7" s="10">
+        <v>0</v>
       </c>
       <c r="I7" s="31" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
+      <c r="J7" s="31" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsErrors" dxfId="4" priority="1">
+    <cfRule type="containsErrors" dxfId="3" priority="1">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€/m)" prompt="Capacity-independent investment costs for pipe/cable to transmit that commodity." sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable invest costs (€/kW/m)" prompt="Capacity-dependent investment costs for transmission capacity of a commodity from one vertex to another." sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Purchase costs (€/kWh)" prompt="Cost for buying that commodity at source vertices, if any exist in the vertex_shapefile." sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed loss fraction (kW/m)" prompt="Powerflow-independent loss of energy per meter of transmission length through the network. The fixed loss is calculated by (length * loss-fix)." sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable power loss (1/kW/m)" prompt="Relative loss term, dependent on input power flow through a &quot;pipe&quot;:_x000a_Ingoing power flow per edge is multiplied by (1 - length * loss-var)" sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Maximum possible transmission capacity per edge." sqref="H1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum allowed generation" prompt="Limits the net amount of generation of this commodity (e.g. CO2). Note that processes that consume a commodity (e.g. CCS) can reduce the net amount." sqref="I1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable invest costs (€/kW/m)" prompt="Capacity-dependent investment costs for transmission capacity of a commodity from one vertex to another." sqref="D1:E1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Purchase costs (€/kWh)" prompt="Cost for buying that commodity at source vertices, if any exist in the vertex_shapefile." sqref="F1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed loss fraction (kW/m)" prompt="Powerflow-independent loss of energy per meter of transmission length through the network. The fixed loss is calculated by (length * loss-fix)." sqref="G1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable power loss (1/kW/m)" prompt="Relative loss term, dependent on input power flow through a &quot;pipe&quot;:_x000a_Ingoing power flow per edge is multiplied by (1 - length * loss-var)" sqref="H1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Maximum possible transmission capacity per edge." sqref="I1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum allowed generation" prompt="Limits the net amount of generation of this commodity (e.g. CO2). Note that processes that consume a commodity (e.g. CCS) can reduce the net amount." sqref="J1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1500,25 +1528,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="35"/>
-    <col min="3" max="4" width="11.42578125" style="3"/>
-    <col min="5" max="6" width="11.42578125" style="35"/>
-    <col min="7" max="16384" width="11.42578125" style="3"/>
+    <col min="3" max="5" width="11.42578125" style="3"/>
+    <col min="6" max="7" width="11.42578125" style="35"/>
+    <col min="8" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1529,19 +1557,22 @@
         <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="F1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="G1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="I1" s="36" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1554,17 +1585,20 @@
       <c r="D2" s="3">
         <v>0</v>
       </c>
-      <c r="E2" s="35">
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="35">
         <v>15000</v>
       </c>
-      <c r="F2" s="35">
+      <c r="G2" s="35">
         <v>600000</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -1577,17 +1611,20 @@
       <c r="D3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="35">
         <v>15000</v>
       </c>
-      <c r="F3" s="35">
+      <c r="G3" s="35">
         <v>600000</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -1600,17 +1637,20 @@
       <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="35">
+      <c r="E4" s="3">
         <v>0</v>
       </c>
       <c r="F4" s="35">
+        <v>0</v>
+      </c>
+      <c r="G4" s="35">
         <v>6000</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -1623,17 +1663,20 @@
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="35">
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="35">
         <v>1000</v>
       </c>
-      <c r="F5" s="35">
+      <c r="G5" s="35">
         <v>150000</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1646,17 +1689,20 @@
       <c r="D6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="35">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="35">
         <v>1000</v>
       </c>
-      <c r="F6" s="35">
+      <c r="G6" s="35">
         <v>400000</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -1669,17 +1715,20 @@
       <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="35">
         <v>5000</v>
       </c>
-      <c r="F7" s="35">
+      <c r="G7" s="35">
         <v>150000</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -1692,17 +1741,20 @@
       <c r="D8" s="3">
         <v>0</v>
       </c>
-      <c r="E8" s="35">
+      <c r="E8" s="3">
         <v>0</v>
       </c>
       <c r="F8" s="35">
+        <v>0</v>
+      </c>
+      <c r="G8" s="35">
         <v>6000</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -1715,23 +1767,27 @@
       <c r="D9" s="3">
         <v>0</v>
       </c>
-      <c r="E9" s="35">
+      <c r="E9" s="3">
         <v>0</v>
       </c>
       <c r="F9" s="35">
         <v>0</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="G9" s="35">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€)" prompt="Up-front investment for building a plant, independent of size._x000a_Has value zero mainly for small-scale technologies." sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific investment costs (€/kW)" prompt="Size-dependent part for building a plant." sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable costs (€/kWh)" prompt="Operational costs to produce one unit of output, excluding fuel costs. Has value zero e.g. for PV or wind turbines (or if no sources are available)." sqref="D1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum capacity (kW)" prompt="Smallest size a plant is typically available in. Has value zero for domestic technologies." sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Biggest capacity a plant typically is available in." sqref="F1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable costs (€/kWh)" prompt="Operational costs to produce one unit of output, excluding fuel costs. Has value zero e.g. for PV or wind turbines (or if no sources are available)." sqref="E1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum capacity (kW)" prompt="Smallest size a plant is typically available in. Has value zero for domestic technologies." sqref="F1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Biggest capacity a plant typically is available in." sqref="G1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific fixed costs (€/kW)" prompt="Size-dependent part for mainting a plant." sqref="D1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2137,10 +2193,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>EXACT("In", INDIRECT("Z"&amp;ROW()&amp;"S3",FALSE()))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2398,7 +2454,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>